<commit_message>
thay doi thu vien datetime
</commit_message>
<xml_diff>
--- a/src/assets/template-excel/Template_Users_Coupon.xlsx
+++ b/src/assets/template-excel/Template_Users_Coupon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhpn/Documents/Developer/TVO/NCB_smart/src/assets/template-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a78c14ff320baf35/Tài liệu/Angular/NCB_smart/src/assets/template-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C4759-BB40-8E46-B687-822ECA99B12A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FC0C4759-BB40-8E46-B687-822ECA99B12A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2630BD69-0241-4373-A24C-649BDDA4D027}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="list_status">'Status map'!$A$1:$A$40</definedName>
     <definedName name="status">'Status map'!$A$1:$A$42</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -293,16 +293,16 @@
     <t>userCif</t>
   </si>
   <si>
-    <t>Nguyen Van A</t>
-  </si>
-  <si>
     <t>Cif123456</t>
   </si>
   <si>
-    <t>Nguyen Van B</t>
-  </si>
-  <si>
     <t>Cif654321</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>NguyenVanB</t>
   </si>
 </sst>
 </file>
@@ -645,22 +645,22 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="1023" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="25.375" customWidth="1"/>
+    <col min="7" max="7" width="22.375" customWidth="1"/>
+    <col min="8" max="1023" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -668,12 +668,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -681,12 +681,12 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -694,7 +694,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -703,7 +703,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -712,7 +712,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
@@ -721,7 +721,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
@@ -730,7 +730,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -739,7 +739,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -748,7 +748,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -757,7 +757,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -786,16 +786,16 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="56.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="39" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="10.83203125" customWidth="1"/>
+    <col min="5" max="1025" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="str">
         <f t="shared" ref="A1:A41" si="0">CONCATENATE(B1,C1,D1)</f>
         <v>Awaiting to verify:100</v>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Verified:200</v>
@@ -825,7 +825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Picking:201</v>
@@ -840,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Pickup failed:202</v>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>On the way to drop-off:203</v>
@@ -870,7 +870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Processing at warehouse:210</v>
@@ -885,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Ready to ship at warehouse:211</v>
@@ -900,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out of stock:212</v>
@@ -915,7 +915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Hold in warehouse:213</v>
@@ -930,7 +930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Awaiting to sourcing:220</v>
@@ -945,7 +945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cross border processing:230</v>
@@ -960,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Received at origin facility:231</v>
@@ -975,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Departed at origin facility:232</v>
@@ -990,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cross border transit:233</v>
@@ -1005,7 +1005,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Customs onhold:234</v>
@@ -1020,7 +1020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Customs cleared:235</v>
@@ -1035,7 +1035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Received at desitination facility:236</v>
@@ -1050,7 +1050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Departed at desitination facility:237</v>
@@ -1065,7 +1065,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Shipped:300</v>
@@ -1080,7 +1080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>In-transit:304</v>
@@ -1095,7 +1095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out for delivery:310</v>
@@ -1110,7 +1110,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out of delivery:400</v>
@@ -1125,7 +1125,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Awaiting for Re-delivery:410</v>
@@ -1140,7 +1140,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Return processing:420</v>
@@ -1155,7 +1155,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Return approved:430</v>
@@ -1170,7 +1170,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Returning:500</v>
@@ -1185,7 +1185,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Out of return:510</v>
@@ -1200,7 +1200,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Return refused:511</v>
@@ -1215,7 +1215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Awaiting receive at facility:520</v>
@@ -1230,7 +1230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Return to orgin facility:530</v>
@@ -1245,7 +1245,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Returned:600</v>
@@ -1260,7 +1260,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Destroy at destination:605</v>
@@ -1275,7 +1275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Returned at orgin facility:610</v>
@@ -1290,7 +1290,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cancelled by sellers:700</v>
@@ -1305,7 +1305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cancelled by operator:701</v>
@@ -1320,7 +1320,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cancelled by partner:702</v>
@@ -1335,7 +1335,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cancelled by system:703</v>
@@ -1350,7 +1350,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Pending for audit status:704</v>
@@ -1365,7 +1365,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Cancelled at warehouse:705</v>
@@ -1380,7 +1380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Delivered:800</v>
@@ -1395,7 +1395,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Closed:900</v>

</xml_diff>